<commit_message>
added images and results
</commit_message>
<xml_diff>
--- a/results/Runtimeresults.xlsx
+++ b/results/Runtimeresults.xlsx
@@ -60,22 +60,10 @@
     <t>average</t>
   </si>
   <si>
-    <t>Matrix Condensation Average Execution time (s)</t>
-  </si>
-  <si>
-    <t>Gaussian Elimination Average Execution time (s)</t>
-  </si>
-  <si>
-    <t>Gaussian Elimination Scalapack Average Execution time (s)</t>
-  </si>
-  <si>
     <t>Matrix Condensation Speed-up</t>
   </si>
   <si>
     <t>Gaussian Elimination Speed-up</t>
-  </si>
-  <si>
-    <t>Gaussian Elimination Scalapack Speed-up</t>
   </si>
   <si>
     <t>Matrix Condensation Average Communication time (s)</t>
@@ -88,6 +76,18 @@
   </si>
   <si>
     <t>Gaussian Elimination Distribution time (s)</t>
+  </si>
+  <si>
+    <t>Gaussian Elimination Scalapack (Blocksize=1) Speed-up</t>
+  </si>
+  <si>
+    <t>Matrix Condensation Execution time (s) After Averaging 5 runs</t>
+  </si>
+  <si>
+    <t>Gaussian Elimination Execution time (s) After Averaging 5 runs</t>
+  </si>
+  <si>
+    <t>Gaussian Elimination Using SCaLAPACK (Blocksize = 1) Execution time (s) After Averaging 5 runs</t>
   </si>
 </sst>
 </file>
@@ -314,22 +314,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -350,7 +338,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -645,79 +645,79 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="18"/>
+      <c r="N2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
-      <c r="N2" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="22"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="18"/>
     </row>
     <row r="3" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="25"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="25"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="21"/>
     </row>
     <row r="4" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="19"/>
-      <c r="N4" s="15" t="s">
+      <c r="E4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
+      <c r="N4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="19"/>
+      <c r="O4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="26"/>
     </row>
     <row r="5" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D5" s="16"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="1">
         <v>1</v>
       </c>
@@ -742,7 +742,7 @@
       <c r="L5" s="1">
         <v>128</v>
       </c>
-      <c r="N5" s="16"/>
+      <c r="N5" s="23"/>
       <c r="O5" s="1">
         <v>1</v>
       </c>
@@ -772,28 +772,28 @@
       <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>0.2034</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>0.1038</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <v>6.0400000000000002E-2</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="5">
         <v>3.9E-2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="5">
         <v>2.9600000000000001E-2</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="5">
         <v>0.55120000000000002</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="5">
         <v>1.4343999999999999</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="5">
         <v>3.0762</v>
       </c>
       <c r="N6" s="1" t="s">
@@ -836,28 +836,28 @@
       <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>1.9319999999999999</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>0.98419999999999996</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
         <v>0.42680000000000001</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
         <v>0.2412</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="5">
         <v>0.1522</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="5">
         <v>0.63939999999999997</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="5">
         <v>1.488</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="5">
         <v>3.1496</v>
       </c>
       <c r="N7" s="1" t="s">
@@ -900,28 +900,28 @@
       <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>8.4052000000000007</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <v>4.5228000000000002</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
         <v>1.835</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="5">
         <v>1.1237999999999999</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="5">
         <v>0.82220000000000004</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="5">
         <v>0.84760000000000002</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="5">
         <v>1.6812</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="5">
         <v>3.2946</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -964,28 +964,28 @@
       <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>20.9512</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="5">
         <v>11.3832</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="5">
         <v>5.2746000000000004</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="5">
         <v>3.6152000000000002</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="5">
         <v>3.0596000000000001</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="5">
         <v>1.4572000000000001</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="5">
         <v>1.9588000000000001</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="5">
         <v>3.5421999999999998</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -1028,28 +1028,28 @@
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>41.5336</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="5">
         <v>22.635999999999999</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="5">
         <v>10.95</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="5">
         <v>7.7178000000000004</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="5">
         <v>6.7576000000000001</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="5">
         <v>3.2475999999999998</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="5">
         <v>2.3565999999999998</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="5">
         <v>3.9367999999999999</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -1092,28 +1092,28 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="5">
         <v>71.923199999999994</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="5">
         <v>39.427999999999997</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="5">
         <v>19.414999999999999</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="5">
         <v>13.779</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="5">
         <v>12.3908</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="5">
         <v>6.1574</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="5">
         <v>3.7342</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="5">
         <v>5.2123999999999997</v>
       </c>
       <c r="N11" s="1" t="s">
@@ -1156,28 +1156,28 @@
       <c r="D12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="5">
         <v>114.477</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="5">
         <v>62.6678</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="5">
         <v>31.147600000000001</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="5">
         <v>22.409199999999998</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="5">
         <v>20.073599999999999</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="5">
         <v>10.1492</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="5">
         <v>5.5750000000000002</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="5">
         <v>5.9775999999999998</v>
       </c>
       <c r="N12" s="1" t="s">
@@ -1220,28 +1220,28 @@
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="5">
         <v>170.80099999999999</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="5">
         <v>94.060599999999994</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="5">
         <v>46.853000000000002</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="5">
         <v>33.726599999999998</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="5">
         <v>31.2834</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="5">
         <v>15.742599999999999</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="5">
         <v>8.1620000000000008</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="5">
         <v>7.173</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1318,79 +1318,79 @@
       </c>
     </row>
     <row r="19" spans="4:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="18"/>
+      <c r="N19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="N19" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
     </row>
     <row r="20" spans="4:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
     </row>
     <row r="21" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="N21" s="14" t="s">
+      <c r="E21" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="N21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O21" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
+      <c r="O21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
     </row>
     <row r="22" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D22" s="14"/>
+      <c r="D22" s="15"/>
       <c r="E22" s="3">
         <v>1</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="L22" s="3">
         <v>128</v>
       </c>
-      <c r="N22" s="14"/>
+      <c r="N22" s="15"/>
       <c r="O22" s="7">
         <v>1</v>
       </c>
@@ -1445,28 +1445,28 @@
       <c r="D23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="6">
         <v>0.19339999999999999</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="6">
         <v>0.1062</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="6">
         <v>6.6199999999999995E-2</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="6">
         <v>4.7E-2</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="6">
         <v>4.0599999999999997E-2</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="6">
         <v>3.6223999999999998</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="6">
         <v>9.2904</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="6">
         <v>11.1374</v>
       </c>
       <c r="N23" s="7" t="s">
@@ -1508,28 +1508,28 @@
       <c r="D24" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="6">
         <v>1.8340000000000001</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F24" s="6">
         <v>0.97840000000000005</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="6">
         <v>0.43840000000000001</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="6">
         <v>0.26040000000000002</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="6">
         <v>0.1812</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="6">
         <v>4.1539999999999999</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="6">
         <v>15.538399999999999</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="6">
         <v>22.991</v>
       </c>
       <c r="N24" s="7" t="s">
@@ -1571,28 +1571,28 @@
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="6">
         <v>8.1004000000000005</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="6">
         <v>4.4733999999999998</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="6">
         <v>1.8495999999999999</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="6">
         <v>1.1606000000000001</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="6">
         <v>0.88739999999999997</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="6">
         <v>4.5556000000000001</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="6">
         <v>19.070799999999998</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="6">
         <v>35.095199999999998</v>
       </c>
       <c r="N25" s="7" t="s">
@@ -1634,28 +1634,28 @@
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="6">
         <v>20.367000000000001</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="6">
         <v>11.2768</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="6">
         <v>5.2746000000000004</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="6">
         <v>3.6640000000000001</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="6">
         <v>3.1467999999999998</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="6">
         <v>5.2957999999999998</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="6">
         <v>21.971599999999999</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="6">
         <v>44.356999999999999</v>
       </c>
       <c r="N26" s="7" t="s">
@@ -1697,28 +1697,28 @@
       <c r="D27" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="6">
         <v>40.505400000000002</v>
       </c>
-      <c r="F27" s="4">
+      <c r="F27" s="6">
         <v>22.390999999999998</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="6">
         <v>10.9184</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="6">
         <v>7.7862</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="6">
         <v>6.9917999999999996</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="6">
         <v>7.2535999999999996</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="6">
         <v>24.270199999999999</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="6">
         <v>55.069800000000001</v>
       </c>
       <c r="N27" s="7" t="s">
@@ -1760,28 +1760,28 @@
       <c r="D28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="6">
         <v>70.361199999999997</v>
       </c>
-      <c r="F28" s="4">
+      <c r="F28" s="6">
         <v>39.173999999999999</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="6">
         <v>19.405999999999999</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="6">
         <v>13.9398</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="6">
         <v>12.5322</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="6">
         <v>10.2332</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="6">
         <v>26.38</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="6">
         <v>59.7254</v>
       </c>
       <c r="N28" s="7" t="s">
@@ -1823,28 +1823,28 @@
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="6">
         <v>111.92700000000001</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F29" s="6">
         <v>62.306399999999996</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="6">
         <v>31.032399999999999</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="6">
         <v>22.696200000000001</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="6">
         <v>21.1934</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="6">
         <v>14.401400000000001</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="6">
         <v>29.234999999999999</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="6">
         <v>67.774199999999993</v>
       </c>
       <c r="N29" s="7" t="s">
@@ -1886,28 +1886,28 @@
       <c r="D30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="6">
         <v>167.43700000000001</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="6">
         <v>94.219399999999993</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="6">
         <v>47.080599999999997</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="6">
         <v>34.265999999999998</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="6">
         <v>31.7562</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="6">
         <v>19.485800000000001</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="6">
         <v>31.904199999999999</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="6">
         <v>75.152600000000007</v>
       </c>
       <c r="N30" s="7" t="s">
@@ -1982,79 +1982,79 @@
       </c>
     </row>
     <row r="35" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D35" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="N35" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
-      <c r="Q35" s="26"/>
-      <c r="R35" s="26"/>
-      <c r="S35" s="26"/>
-      <c r="T35" s="26"/>
-      <c r="U35" s="26"/>
-      <c r="V35" s="26"/>
+      <c r="D35" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="18"/>
+      <c r="N35" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="O35" s="14"/>
+      <c r="P35" s="14"/>
+      <c r="Q35" s="14"/>
+      <c r="R35" s="14"/>
+      <c r="S35" s="14"/>
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
     </row>
     <row r="36" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
-      <c r="J36" s="26"/>
-      <c r="K36" s="26"/>
-      <c r="L36" s="26"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
-      <c r="Q36" s="26"/>
-      <c r="R36" s="26"/>
-      <c r="S36" s="26"/>
-      <c r="T36" s="26"/>
-      <c r="U36" s="26"/>
-      <c r="V36" s="26"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="21"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
     </row>
     <row r="37" spans="4:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="N37" s="14" t="s">
+      <c r="E37" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="N37" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O37" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
-      <c r="V37" s="14"/>
+      <c r="O37" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
+      <c r="S37" s="15"/>
+      <c r="T37" s="15"/>
+      <c r="U37" s="15"/>
+      <c r="V37" s="15"/>
     </row>
     <row r="38" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D38" s="14"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="3">
         <v>1</v>
       </c>
@@ -2079,7 +2079,7 @@
       <c r="L38" s="3">
         <v>128</v>
       </c>
-      <c r="N38" s="14"/>
+      <c r="N38" s="15"/>
       <c r="O38" s="3">
         <v>1</v>
       </c>
@@ -2109,28 +2109,28 @@
       <c r="D39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="6">
         <v>1.6172</v>
       </c>
-      <c r="F39" s="4">
+      <c r="F39" s="6">
         <v>1.1886000000000001</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="6">
         <v>1.0098</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="6">
         <v>0.94479999999999997</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="6">
         <v>0.996</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="6">
         <v>1.3311999999999999</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="6">
         <v>1.6866000000000001</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="6">
         <v>2.3481999999999998</v>
       </c>
       <c r="N39" s="7" t="s">
@@ -2173,28 +2173,28 @@
       <c r="D40" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="6">
         <v>7.6151999999999997</v>
       </c>
-      <c r="F40" s="4">
+      <c r="F40" s="6">
         <v>5.3868</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="6">
         <v>4.1471999999999998</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="6">
         <v>3.536</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="6">
         <v>3.3576000000000001</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="6">
         <v>3.9441999999999999</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="6">
         <v>4.4471999999999996</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="6">
         <v>5.3011999999999997</v>
       </c>
       <c r="N40" s="7" t="s">
@@ -2237,28 +2237,28 @@
       <c r="D41" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="6">
         <v>21.049199999999999</v>
       </c>
-      <c r="F41" s="4">
+      <c r="F41" s="6">
         <v>14.132400000000001</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="6">
         <v>10.284599999999999</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="6">
         <v>8.4722000000000008</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="6">
         <v>7.7808000000000002</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="6">
         <v>8.5236000000000001</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="6">
         <v>8.9434000000000005</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="6">
         <v>10.1602</v>
       </c>
       <c r="N41" s="7" t="s">
@@ -2301,28 +2301,28 @@
       <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="6">
         <v>43.216999999999999</v>
       </c>
-      <c r="F42" s="4">
+      <c r="F42" s="6">
         <v>28.5212</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="6">
         <v>19.906400000000001</v>
       </c>
-      <c r="H42" s="4">
+      <c r="H42" s="6">
         <v>16.663799999999998</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="6">
         <v>15.1816</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="6">
         <v>15.195</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="6">
         <v>15.4236</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="6">
         <v>17.044799999999999</v>
       </c>
       <c r="N42" s="7" t="s">
@@ -2365,28 +2365,28 @@
       <c r="D43" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E43" s="6">
         <v>77.984800000000007</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F43" s="6">
         <v>49.323</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="6">
         <v>33.987400000000001</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="6">
         <v>28.241399999999999</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="6">
         <v>25.7898</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="6">
         <v>24.476400000000002</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="6">
         <v>24.3308</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="6">
         <v>25.578399999999998</v>
       </c>
       <c r="N43" s="7" t="s">
@@ -2429,28 +2429,28 @@
       <c r="D44" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="4">
+      <c r="E44" s="6">
         <v>126.188</v>
       </c>
-      <c r="F44" s="4">
+      <c r="F44" s="6">
         <v>77.703199999999995</v>
       </c>
-      <c r="G44" s="4">
+      <c r="G44" s="6">
         <v>52.225200000000001</v>
       </c>
-      <c r="H44" s="4">
+      <c r="H44" s="6">
         <v>43.017400000000002</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="6">
         <v>39.367600000000003</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="6">
         <v>37.092399999999998</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="6">
         <v>34.857999999999997</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="6">
         <v>36.543199999999999</v>
       </c>
       <c r="N44" s="7" t="s">
@@ -2493,28 +2493,28 @@
       <c r="D45" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="4">
+      <c r="E45" s="6">
         <v>187.74600000000001</v>
       </c>
-      <c r="F45" s="4">
+      <c r="F45" s="6">
         <v>115.55200000000001</v>
       </c>
-      <c r="G45" s="4">
+      <c r="G45" s="6">
         <v>76.586600000000004</v>
       </c>
-      <c r="H45" s="4">
+      <c r="H45" s="6">
         <v>62.2714</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45" s="6">
         <v>56.834600000000002</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="6">
         <v>50.593600000000002</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="6">
         <v>49.9148</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="6">
         <v>49.0486</v>
       </c>
       <c r="N45" s="7" t="s">
@@ -2557,28 +2557,28 @@
       <c r="D46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="4">
+      <c r="E46" s="6">
         <v>268.68400000000003</v>
       </c>
-      <c r="F46" s="4">
+      <c r="F46" s="6">
         <v>163.05799999999999</v>
       </c>
-      <c r="G46" s="4">
+      <c r="G46" s="6">
         <v>105.80200000000001</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="6">
         <v>85.333399999999997</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46" s="6">
         <v>78.465400000000002</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="6">
         <v>69.436800000000005</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="6">
         <v>64.597999999999999</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="6">
         <v>63.644599999999997</v>
       </c>
       <c r="N46" s="7" t="s">
@@ -2655,79 +2655,79 @@
       </c>
     </row>
     <row r="53" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D53" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="22"/>
-      <c r="N53" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="O53" s="26"/>
-      <c r="P53" s="26"/>
-      <c r="Q53" s="26"/>
-      <c r="R53" s="26"/>
-      <c r="S53" s="26"/>
-      <c r="T53" s="26"/>
-      <c r="U53" s="26"/>
-      <c r="V53" s="26"/>
+      <c r="D53" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="18"/>
+      <c r="N53" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="O53" s="14"/>
+      <c r="P53" s="14"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
+      <c r="V53" s="14"/>
     </row>
     <row r="54" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D54" s="23"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="25"/>
-      <c r="N54" s="26"/>
-      <c r="O54" s="26"/>
-      <c r="P54" s="26"/>
-      <c r="Q54" s="26"/>
-      <c r="R54" s="26"/>
-      <c r="S54" s="26"/>
-      <c r="T54" s="26"/>
-      <c r="U54" s="26"/>
-      <c r="V54" s="26"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="21"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
+      <c r="V54" s="14"/>
     </row>
     <row r="55" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="19"/>
-      <c r="N55" s="14" t="s">
+      <c r="E55" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="25"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="25"/>
+      <c r="I55" s="25"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="25"/>
+      <c r="L55" s="26"/>
+      <c r="N55" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O55" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="P55" s="14"/>
-      <c r="Q55" s="14"/>
-      <c r="R55" s="14"/>
-      <c r="S55" s="14"/>
-      <c r="T55" s="14"/>
-      <c r="U55" s="14"/>
-      <c r="V55" s="14"/>
+      <c r="O55" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
+      <c r="S55" s="15"/>
+      <c r="T55" s="15"/>
+      <c r="U55" s="15"/>
+      <c r="V55" s="15"/>
     </row>
     <row r="56" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D56" s="16"/>
+      <c r="D56" s="23"/>
       <c r="E56" s="1">
         <v>1</v>
       </c>
@@ -2752,7 +2752,7 @@
       <c r="L56" s="1">
         <v>128</v>
       </c>
-      <c r="N56" s="14"/>
+      <c r="N56" s="15"/>
       <c r="O56" s="8">
         <v>1</v>
       </c>
@@ -3299,79 +3299,79 @@
       </c>
     </row>
     <row r="75" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D75" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="21"/>
-      <c r="K75" s="21"/>
-      <c r="L75" s="22"/>
-      <c r="N75" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="O75" s="26"/>
-      <c r="P75" s="26"/>
-      <c r="Q75" s="26"/>
-      <c r="R75" s="26"/>
-      <c r="S75" s="26"/>
-      <c r="T75" s="26"/>
-      <c r="U75" s="26"/>
-      <c r="V75" s="26"/>
+      <c r="D75" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="18"/>
+      <c r="N75" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="O75" s="14"/>
+      <c r="P75" s="14"/>
+      <c r="Q75" s="14"/>
+      <c r="R75" s="14"/>
+      <c r="S75" s="14"/>
+      <c r="T75" s="14"/>
+      <c r="U75" s="14"/>
+      <c r="V75" s="14"/>
     </row>
     <row r="76" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D76" s="23"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24"/>
-      <c r="K76" s="24"/>
-      <c r="L76" s="25"/>
-      <c r="N76" s="26"/>
-      <c r="O76" s="26"/>
-      <c r="P76" s="26"/>
-      <c r="Q76" s="26"/>
-      <c r="R76" s="26"/>
-      <c r="S76" s="26"/>
-      <c r="T76" s="26"/>
-      <c r="U76" s="26"/>
-      <c r="V76" s="26"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="21"/>
+      <c r="N76" s="14"/>
+      <c r="O76" s="14"/>
+      <c r="P76" s="14"/>
+      <c r="Q76" s="14"/>
+      <c r="R76" s="14"/>
+      <c r="S76" s="14"/>
+      <c r="T76" s="14"/>
+      <c r="U76" s="14"/>
+      <c r="V76" s="14"/>
     </row>
     <row r="77" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D77" s="15" t="s">
+      <c r="D77" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E77" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="18"/>
-      <c r="L77" s="19"/>
-      <c r="N77" s="14" t="s">
+      <c r="E77" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="25"/>
+      <c r="G77" s="25"/>
+      <c r="H77" s="25"/>
+      <c r="I77" s="25"/>
+      <c r="J77" s="25"/>
+      <c r="K77" s="25"/>
+      <c r="L77" s="26"/>
+      <c r="N77" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O77" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="P77" s="14"/>
-      <c r="Q77" s="14"/>
-      <c r="R77" s="14"/>
-      <c r="S77" s="14"/>
-      <c r="T77" s="14"/>
-      <c r="U77" s="14"/>
-      <c r="V77" s="14"/>
+      <c r="O77" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
     </row>
     <row r="78" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D78" s="16"/>
+      <c r="D78" s="23"/>
       <c r="E78" s="1">
         <v>1</v>
       </c>
@@ -3396,7 +3396,7 @@
       <c r="L78" s="1">
         <v>128</v>
       </c>
-      <c r="N78" s="14"/>
+      <c r="N78" s="15"/>
       <c r="O78" s="8">
         <v>1</v>
       </c>

</xml_diff>